<commit_message>
Removed redundant folders. Minor edits to log spreadsheets
</commit_message>
<xml_diff>
--- a/.assumptions/qualitative_assumptions/assumptions_and_decision_log_template.xlsx
+++ b/.assumptions/qualitative_assumptions/assumptions_and_decision_log_template.xlsx
@@ -4,9 +4,9 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A894292E-3B1D-4C08-B5AA-52A90D96EE28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FF27A59C-2764-40A6-AD4A-668F784AF0E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="856" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="11" r:id="rId1"/>
@@ -18,8 +18,8 @@
     <sheet name="Decisions &amp; Issues Register" sheetId="7" r:id="rId7"/>
     <sheet name="Assumptions log " sheetId="6" r:id="rId8"/>
     <sheet name="Quality &amp; Sensitivity Guide" sheetId="5" r:id="rId9"/>
-    <sheet name="Risk Scoring Guide" sheetId="8" r:id="rId10"/>
-    <sheet name="Ethics Log" sheetId="13" r:id="rId11"/>
+    <sheet name="Ethics Log" sheetId="13" r:id="rId10"/>
+    <sheet name="Risk Scoring Guide" sheetId="8" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Decisions &amp; Issues Register'!$B$10:$L$11</definedName>
@@ -100,10 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="205">
-  <si>
-    <t>This template supports analysis development and production by providing a structured template for documentation</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="206">
   <si>
     <t>While most of the template should be self explanatory, this introductory slide sets out basic guidance on use.</t>
   </si>
@@ -120,28 +117,22 @@
     <t>Summary</t>
   </si>
   <si>
-    <t>Particular Details</t>
-  </si>
-  <si>
     <t>Analysis Overview</t>
   </si>
   <si>
-    <t xml:space="preserve">A table with a series of boxes to be filled in by the owning team which outlines some of the basic model </t>
-  </si>
-  <si>
     <t>Analysis Map</t>
   </si>
   <si>
     <t>A graphical representation of all the inputs into the analysis, what processes they go through and the outputs created by the analysis. These outputs should then, ideally, be linked to planned or ongoing publications.</t>
   </si>
   <si>
-    <t>Roles &amp; Responsibiltiies</t>
+    <t>Roles &amp; Responsibilities</t>
   </si>
   <si>
     <t>Records when somebody took on a governance role and if they reviewed the documentation relevant to the responsibiltiies of the role. Also records past governance ownership to ensure that handovers are recorded.</t>
   </si>
   <si>
-    <t>The guidance for each role to follow and agree to is on the subsequent sheet, labled 'R&amp;R Resources'</t>
+    <t>Guidance about what each assurance role involves and templates to record agreement to carry out that role are on the sheet labelled 'R&amp;R Resources'</t>
   </si>
   <si>
     <t>R&amp;R Resources</t>
@@ -153,7 +144,7 @@
     <t>QA Log</t>
   </si>
   <si>
-    <t>A Table which allows the Analytical Assurer to document the planned Quality Assurance that will occur and confirm that this did, in fact, occur. Also has space for a short summary of the issues the Quality Assurance raised. This information should be described more fully in the decisions and issues register</t>
+    <t>A Table which allows the Analytical Assurer to document planned Quality Assurance and confirm when it is completed. Also has space for a short summary of the issues the Quality Assurance raised. This information should be described more fully in the decisions and issues register</t>
   </si>
   <si>
     <t>Decisions &amp; Issues Register</t>
@@ -165,15 +156,9 @@
     <t>Assumptions Log</t>
   </si>
   <si>
-    <t>This table records the assumptions made regarding the model. These will often be decisions made due to the impossible nature of perfectly representing reality in a model. These assumptions will almost always have a numerical value and an uncertainty interval around this value to demonstrate the degree of uncertainty the team has regarding the validity of the assumption. The assumptions will have a quality rating which, when multiplied by the model's sensitivity to the assumption, forms the risks score. The risk score should inform how resources are allocated to the further research and improvement of the assumptions.</t>
-  </si>
-  <si>
     <t>Quality &amp; Sensitivity Guide</t>
   </si>
   <si>
-    <t>A at-a-glance guide to quality scoring. If there is ever uncertainty about the quality / sensitivity score of an assumption, err on the side of caution and rate it the more risky of the two. That is to say lower quality, higher sensitivity.</t>
-  </si>
-  <si>
     <t>Risk Scoring Guide</t>
   </si>
   <si>
@@ -192,10 +177,15 @@
     <t>Analysis purpose</t>
   </si>
   <si>
-    <t>Owning Team(s)</t>
-  </si>
-  <si>
-    <t>Code Repo Location</t>
+    <t>Owning team(s)</t>
+  </si>
+  <si>
+    <t>Code Repository URL</t>
+  </si>
+  <si>
+    <t>URL of the code repository on Gitlab or Github for the workflow. 
+For multiple repositories, include the URLs for all relevant ones. 
+Put each URL on a new line.</t>
   </si>
   <si>
     <t>List of Stakeholders</t>
@@ -302,13 +292,10 @@
     <t>Methodology document</t>
   </si>
   <si>
-    <t>Publication / Output</t>
+    <t>Publications and Outputs</t>
   </si>
   <si>
     <t>Other relevant research documents</t>
-  </si>
-  <si>
-    <t>Most teams will create process maps or model maps during development</t>
   </si>
   <si>
     <t>Recreating these in Excel can be cumbersome. Images, slides and other formats can be copy-pasted here for ease of reference</t>
@@ -435,259 +422,32 @@
     <t xml:space="preserve">Handover Example </t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">If a handover has occured and the owner of a role changes, please </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">add </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>your name in the sign off box.</t>
+    </r>
+  </si>
+  <si>
     <t>Do not overwrite the existing name</t>
   </si>
   <si>
     <t>Senior Responsible Owner overview</t>
-  </si>
-  <si>
-    <t>Commissioner Overview</t>
-  </si>
-  <si>
-    <t>Analytical Assurer Overview</t>
-  </si>
-  <si>
-    <t>SRO</t>
-  </si>
-  <si>
-    <t>Commisioner Responsibilites</t>
-  </si>
-  <si>
-    <t>Analytical Assurer Responsibilites</t>
-  </si>
-  <si>
-    <t>Responsibility</t>
-  </si>
-  <si>
-    <t>Signed by</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>I agree to review and sign off all key decisions made about the analysis</t>
-  </si>
-  <si>
-    <t>I agree to ensure that sufficent resources and time are allocated to reach the desired level of quality.</t>
-  </si>
-  <si>
-    <t>I agree to communicate key risks, limitations, major assumptions of the analysis and uncertainty associated with the outcomes to users</t>
-  </si>
-  <si>
-    <t>I agree to ensure a high level of understanding of the requirements, scope and context of the analysis, not just for myself, but for the SRO, the Analytical Assurer and the Analyst(s)</t>
-  </si>
-  <si>
-    <t>I agree to quantify input error, major assumptions, limitations and uncertainty mathematically wherever possible.</t>
-  </si>
-  <si>
-    <t>I will ensure that the feedback given by the Quality Assurers is fully documented and reviewed by the modelling team</t>
-  </si>
-  <si>
-    <t>I agree to attempt to mittigate assumptions and limitations by improving analysis design wherever possible.</t>
-  </si>
-  <si>
-    <t>I agree to ensure that the quality assurance process is compliant and appropriate, documenting findings and reviewing them to inform future analysis development.</t>
-  </si>
-  <si>
-    <t>I agree to honestly and openly communicate errors in the model before and after publication to the end users. In particular, if an error is detected post publication, I agree to not withhold information regarding the error from the public and the end users.</t>
-  </si>
-  <si>
-    <t>SRO Documents</t>
-  </si>
-  <si>
-    <t>Commissioner Documents</t>
-  </si>
-  <si>
-    <t>Analytical Assurer Documents</t>
-  </si>
-  <si>
-    <t>Name &amp; Description</t>
-  </si>
-  <si>
-    <t>Created by</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name &amp; Description </t>
-  </si>
-  <si>
-    <t>TODO: Create Word Template</t>
-  </si>
-  <si>
-    <t>QA Plan &amp; Log for [Insert Model Name &amp; Financial Year of Interest]</t>
-  </si>
-  <si>
-    <t>OFFICIAL - SENSITIVE</t>
-  </si>
-  <si>
-    <t>This sheet is a record of past performed quality assurance and future planned quality assurance.
-Each review should be signed off by the Analyitcal Assurer only after
-a) The review has been performed 
-b) The modelling team have recieved the findings of the review
-c) The analytical assurer is sure that the modelling team have understood the findings of the review and have planned  actions based on the review findings.</t>
-  </si>
-  <si>
-    <t>QA Round</t>
-  </si>
-  <si>
-    <t>QA Type</t>
-  </si>
-  <si>
-    <t>Who will perform the review?</t>
-  </si>
-  <si>
-    <t>Start Date</t>
-  </si>
-  <si>
-    <t>Estimated End Date</t>
-  </si>
-  <si>
-    <t>Summary of Findings</t>
-  </si>
-  <si>
-    <t>Sign off By Analytical Assurer</t>
-  </si>
-  <si>
-    <t>Peer Review</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Joh Smith from ASAP (email) </t>
-  </si>
-  <si>
-    <t>01/01/2023 (Agreed on 01/01/2022)</t>
-  </si>
-  <si>
-    <t>01/02/2023 - 01/03/2023</t>
-  </si>
-  <si>
-    <t>Code lacks automated tests
-Assumptions not signed off
-Assumption 001 no longer true in view of new evidence</t>
-  </si>
-  <si>
-    <t>Issue ID</t>
-  </si>
-  <si>
-    <t>Issue</t>
-  </si>
-  <si>
-    <t>Date First Identified</t>
-  </si>
-  <si>
-    <t>Plain English description of issue</t>
-  </si>
-  <si>
-    <t>Impact of issue</t>
-  </si>
-  <si>
-    <t>Status of issue</t>
-  </si>
-  <si>
-    <t>Justification of Status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proof of resolution </t>
-  </si>
-  <si>
-    <t>Reviewed by</t>
-  </si>
-  <si>
-    <t>Assumptions log for [Insert Analysis or Model Name &amp; Financial Year of Interest]</t>
-  </si>
-  <si>
-    <t>Assumption ID</t>
-  </si>
-  <si>
-    <t>Location in code/publication</t>
-  </si>
-  <si>
-    <t>Plain English description of assumption</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Basis for assumption </t>
-  </si>
-  <si>
-    <t>Numerical value of the estimated mean of the assumption</t>
-  </si>
-  <si>
-    <t>Range around the estimated value</t>
-  </si>
-  <si>
-    <t>Estimated distribution</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Links to supporting analysis </t>
-  </si>
-  <si>
-    <t>Documentation dependencies</t>
-  </si>
-  <si>
-    <t>Internally reviewed by</t>
-  </si>
-  <si>
-    <t>Externally reviewed by</t>
-  </si>
-  <si>
-    <t>Date of external review</t>
-  </si>
-  <si>
-    <t>Quality Rating</t>
-  </si>
-  <si>
-    <t>Sensitivity Score</t>
-  </si>
-  <si>
-    <t>Risk Score</t>
-  </si>
-  <si>
-    <t>Green</t>
-  </si>
-  <si>
-    <t>High</t>
-  </si>
-  <si>
-    <t>Low</t>
-  </si>
-  <si>
-    <t>A 1% Change in the tested input creates &lt;0.01% change in the output(s)</t>
-  </si>
-  <si>
-    <t>Amber</t>
-  </si>
-  <si>
-    <t>Medium</t>
-  </si>
-  <si>
-    <t>A 1% Change in the tested input creates a change of between 0.1% and 0.01% in the output(s)</t>
-  </si>
-  <si>
-    <t>Red</t>
-  </si>
-  <si>
-    <t>A 1% Change in the tested input creates &gt;0.1% changein the output(s)</t>
-  </si>
-  <si>
-    <t>Risk should be understood as the product of quality and sensitivity.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The riskiest assumptions and decisions are those with low evidence quality and high impact on final results. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Risk Scoring </t>
-  </si>
-  <si>
-    <t>Med</t>
-  </si>
-  <si>
-    <t>Sensitivity</t>
-  </si>
-  <si>
-    <t>Once risk is calculated, it should be used by teams to ensure that the riskiest assumptions / decisions have the best evidence justifying them.</t>
-  </si>
-  <si>
-    <t>If this is impossible, efforts should be made to reduce the risk by either increasing the quality or reducing the model's sensitity by introducing other independent methodologies.</t>
-  </si>
-  <si>
-    <t>https://uksa.statisticsauthority.gov.uk/the-authority-board/committees/national-statisticians-advisory-committees-and-panels/national-statisticians-data-ethics-advisory-committee/ethics-self-assessment-tool/</t>
   </si>
   <si>
     <r>
@@ -729,6 +489,9 @@
     </r>
   </si>
   <si>
+    <t>Commissioner Overview</t>
+  </si>
+  <si>
     <r>
       <t>The commissioner acts as the liason between the end user and the analytical team. They ensure that the analysis is designed according to the end user need. This means transmitting needs from end users to analysts and concerns and limitations from analysts to end users.</t>
     </r>
@@ -743,51 +506,7 @@
     </r>
   </si>
   <si>
-    <t>I agree to understand and keep up to date with the the strengths, limitations and contexts of the analysis</t>
-  </si>
-  <si>
-    <t>I agree to remain up to date and informed of uncertainties in the analysis and their implications </t>
-  </si>
-  <si>
-    <t>I agree to transmit information regarding the strengths, limitations, context and uncertainties from the analytical team to end users to ensure appropriate analysis development.</t>
-  </si>
-  <si>
-    <t>I agree to transmit information regarding user needs from end users to the analysis team, ensuring that the analysis is developed according to user needs</t>
-  </si>
-  <si>
-    <t>I agree to ensure that sufficent quality assurance happens throughout analysis development and that the analysis complies with the ONS Quality Standard for Analysis</t>
-  </si>
-  <si>
-    <t>I agree to ensure that quality assurance is sufficiently varied, including code review, documentation review, methodological review and discussion with the analysis team to ensure development occurs as planned.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Commissioning document: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>Sets out the question the analysis tries to answer and how this analysis will try to answer it. The commissioning document must be completed before production begins. It should be created in collaboration with end users and the analytical team. The document must set out broad specifications for the analysis including accuracy requirements, delivery timeline and skill gaps that must be addressed before completion.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>QA Plan &amp; Log:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> Sets out the planned quality assurance which should occur before the publication of the analysis. It must include a broad outline of the types of review that will occur (e.g. code review, documentation review, external peer review) as well as indicative dates for when the reviews will occur and who will perform them. Peer reviewers should be contacted well in advance of the start date of the review. The required time, resources and documentation should be discussed with them well in advance of the start date.</t>
-    </r>
-  </si>
-  <si>
-    <t>I agree to ensure that relevant limitations, uncertainties and caveats detected by quality assurance are communicated to end users, both before and after publication.</t>
+    <t>Analytical Assurer Overview</t>
   </si>
   <si>
     <r>
@@ -829,8 +548,76 @@
     </r>
   </si>
   <si>
+    <t>SRO</t>
+  </si>
+  <si>
+    <t>Commisioner Responsibilites</t>
+  </si>
+  <si>
+    <t>Analytical Assurer Responsibilites</t>
+  </si>
+  <si>
+    <t>Responsibility</t>
+  </si>
+  <si>
+    <t>Signed by</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>I agree to review and sign off all key decisions made about the analysis</t>
+  </si>
+  <si>
+    <t>I agree to ensure that sufficent resources and time are allocated to reach the desired level of quality.</t>
+  </si>
+  <si>
+    <t>I agree to ensure that sufficent quality assurance happens throughout analysis development and that the analysis complies with the ONS Quality Standard for Analysis</t>
+  </si>
+  <si>
+    <t>I agree to communicate key risks, limitations, major assumptions of the analysis and uncertainty associated with the outcomes to users</t>
+  </si>
+  <si>
+    <t>I agree to ensure a high level of understanding of the requirements, scope and context of the analysis, not just for myself, but for the SRO, the Analytical Assurer and the Analyst(s)</t>
+  </si>
+  <si>
+    <t>I agree to ensure that quality assurance is sufficiently varied, including code review, documentation review, methodological review and discussion with the analysis team to ensure development occurs as planned.</t>
+  </si>
+  <si>
+    <t>I agree to quantify input error, major assumptions, limitations and uncertainty mathematically wherever possible.</t>
+  </si>
+  <si>
+    <t>I agree to understand and keep up to date with the the strengths, limitations and contexts of the analysis</t>
+  </si>
+  <si>
+    <t>I will ensure that the feedback given by the Quality Assurers is fully documented and reviewed by the modelling team</t>
+  </si>
+  <si>
+    <t>I agree to attempt to mittigate assumptions and limitations by improving analysis design wherever possible.</t>
+  </si>
+  <si>
+    <t>I agree to remain up to date and informed of uncertainties in the analysis and their implications </t>
+  </si>
+  <si>
+    <t>I agree to ensure that relevant limitations, uncertainties and caveats detected by quality assurance are communicated to end users, both before and after publication.</t>
+  </si>
+  <si>
+    <t>I agree to ensure that the quality assurance process is compliant and appropriate, documenting findings and reviewing them to inform future analysis development.</t>
+  </si>
+  <si>
+    <t>I agree to transmit information regarding the strengths, limitations, context and uncertainties from the analytical team to end users to ensure appropriate analysis development.</t>
+  </si>
+  <si>
+    <t>I agree to honestly and openly communicate errors in the model before and after publication to the end users. In particular, if an error is detected post publication, I agree to not withhold information regarding the error from the public and the end users.</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">If a handover has occured and the owner of a role changes, please </t>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">I agree to communicate the concerns of my analysis team to the commissioner. These concerns can include quality, timeline and feasability concerns. </t>
     </r>
     <r>
       <rPr>
@@ -839,7 +626,33 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
       </rPr>
-      <t xml:space="preserve">add </t>
+      <t>It is not acceptable for me to ignore the concerns of the analysis team.</t>
+    </r>
+  </si>
+  <si>
+    <t>I agree to transmit information regarding user needs from end users to the analysis team, ensuring that the analysis is developed according to user needs</t>
+  </si>
+  <si>
+    <t>SRO Documents</t>
+  </si>
+  <si>
+    <t>Commissioner Documents</t>
+  </si>
+  <si>
+    <t>Analytical Assurer Documents</t>
+  </si>
+  <si>
+    <t>Name &amp; Description</t>
+  </si>
+  <si>
+    <t>Created by</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name &amp; Description </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Commissioning document: </t>
     </r>
     <r>
       <rPr>
@@ -847,8 +660,75 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>your name in the sign off box.</t>
+      <t>Sets out the question the analysis tries to answer and how this analysis will try to answer it. The commissioning document must be completed before production begins. It should be created in collaboration with end users and the analytical team. The document must set out broad specifications for the analysis including accuracy requirements, delivery timeline and skill gaps that must be addressed before completion.</t>
     </r>
+  </si>
+  <si>
+    <t>TODO: Create Word Template</t>
+  </si>
+  <si>
+    <r>
+      <t>QA Plan &amp; Log:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> Sets out the planned quality assurance which should occur before the publication of the analysis. It must include a broad outline of the types of review that will occur (e.g. code review, documentation review, external peer review) as well as indicative dates for when the reviews will occur and who will perform them. Peer reviewers should be contacted well in advance of the start date of the review. The required time, resources and documentation should be discussed with them well in advance of the start date.</t>
+    </r>
+  </si>
+  <si>
+    <t>QA Plan &amp; Log for [Insert Analysis Name &amp; Financial Year of Interest]</t>
+  </si>
+  <si>
+    <t>OFFICIAL - SENSITIVE</t>
+  </si>
+  <si>
+    <t>This sheet is a record of past performed quality assurance and future planned quality assurance.
+Each review should be signed off by the Analyitcal Assurer only after
+a) The review has been performed 
+b) The analysis team have recrived the findings of the review
+c) The analytical assurer is sure that the analysis team have understood the findings of the review and have planned  actions based on the review findings.</t>
+  </si>
+  <si>
+    <t>QA Round</t>
+  </si>
+  <si>
+    <t>QA Type</t>
+  </si>
+  <si>
+    <t>Who will perform the review?</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>Estimated End Date</t>
+  </si>
+  <si>
+    <t>Summary of Findings</t>
+  </si>
+  <si>
+    <t>Sign off By Analytical Assurer</t>
+  </si>
+  <si>
+    <t>Peer Review</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joh Smith from ASAP (email) </t>
+  </si>
+  <si>
+    <t>01/01/2023 (Agreed on 01/01/2022)</t>
+  </si>
+  <si>
+    <t>01/02/2023 - 01/03/2023</t>
+  </si>
+  <si>
+    <t>Code lacks automated tests
+Assumptions not signed off
+Assumption 001 no longer true in view of new evidence</t>
   </si>
   <si>
     <t>Issues register for [Insert Analysis Name &amp; Financial Year of Interest]</t>
@@ -859,9 +739,111 @@
 If issues are resolved, they can be evidenced by linking to the relevant place in the analysis where the error, issue or decision impacts.</t>
   </si>
   <si>
+    <t>Issue ID</t>
+  </si>
+  <si>
+    <t>Issue</t>
+  </si>
+  <si>
+    <t>Date First Identified</t>
+  </si>
+  <si>
+    <t>Plain English description of issue</t>
+  </si>
+  <si>
+    <t>Impact of issue</t>
+  </si>
+  <si>
+    <t>Status of issue</t>
+  </si>
+  <si>
+    <t>Justification of Status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proof of resolution </t>
+  </si>
+  <si>
+    <t>Reviewed by</t>
+  </si>
+  <si>
+    <t>Assumptions log for [Insert Analysis or Model Name &amp; Financial Year of Interest]</t>
+  </si>
+  <si>
     <t>Assumptions are made whenever data enters the analysis, a process is applied to data, or an interpretation of the data occurs.
 Most analysis will make dozens of assumptions for even small, simple workflows. Assumptions are often implicit - we recommend holding a workshop in the team to surface them.
 A good place to start is the assumption that the input data is representative - this can be risk scored, impact scored and tested against known populations to understand how representative your inputs are</t>
+  </si>
+  <si>
+    <t>Assumption ID</t>
+  </si>
+  <si>
+    <t>Location in code/publication</t>
+  </si>
+  <si>
+    <t>Plain English description of assumption</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basis for assumption </t>
+  </si>
+  <si>
+    <t>Numerical value of the estimated mean of the assumption</t>
+  </si>
+  <si>
+    <t>Range around the estimated value</t>
+  </si>
+  <si>
+    <t>Estimated distribution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Links to supporting analysis </t>
+  </si>
+  <si>
+    <t>Documentation dependencies</t>
+  </si>
+  <si>
+    <t>Internally reviewed by</t>
+  </si>
+  <si>
+    <t>Externally reviewed by</t>
+  </si>
+  <si>
+    <t>Date of external review</t>
+  </si>
+  <si>
+    <t>Quality Rating</t>
+  </si>
+  <si>
+    <t>Sensitivity Score</t>
+  </si>
+  <si>
+    <t>Risk Score</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Assumption RAG Quality rating. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The quality of an assumption measures both how certain and how robust the assumption is and how appropriate it is for its intended use.
+We would consider a published data source data to be very robust,  but if it needs to be transformed significantly to fit the analysisl, the quality rating would be downgraded.
+You may want to lower the quality rating if it is not possible to get technical sign-off for the assumptions (e.g. lack of technical knowledge).
+You should also lower the quality if the confidence interval is likely to be wide (i.e. you wouldn't be surprised if the value was 50% different) - in this case, you should rank it as Amber / Red.</t>
+    </r>
   </si>
   <si>
     <t>Assumptions are usually Green if:
@@ -869,22 +851,6 @@
 Methodology is robust. 
 There are no or few transformations, or transformation methodology is also fully verified and robust.
 Data is current, and signed off by experts. Small confidence intervals.</t>
-  </si>
-  <si>
-    <t>Assumptions are usually Amber if:
-The methodology  is robust but based on limited data;
-Data required significant transformation to fit the model;
-Confidence intervals are quite wide;
-Data has not been reviewed recently.</t>
-  </si>
-  <si>
-    <t>Assumptions are usually Red if:
-Unclear/unreliable data source or no data source provided. 
-Based on limited data and methodology not robust. 
-Data is not current. Confidence interval wide/unknown.</t>
-  </si>
-  <si>
-    <t>An assumption is also sensitive if it changes the direction / commentary of the output.</t>
   </si>
   <si>
     <r>
@@ -907,55 +873,89 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Assumption RAG Quality rating. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>The quality of an assumption measures both how certain and how robust the assumption is and how appropriate it is for its intended use.
-We would consider a published data source data to be very robust,  but if it needs to be transformed significantly to fit the analysisl, the quality rating would be downgraded.
-You may want to lower the quality rating if it is not possible to get technical sign-off for the assumptions (e.g. lack of technical knowledge).
-You should also lower the quality if the confidence interval is likely to be wide (i.e. you wouldn't be surprised if the value was 50% different) - in this case, you should rank it as Amber / Red.</t>
-    </r>
+    <t>A 1% Change in the tested input creates &lt;0.01% change in the output(s)</t>
+  </si>
+  <si>
+    <t>Amber</t>
+  </si>
+  <si>
+    <t>Assumptions are usually Amber if:
+The methodology  is robust but based on limited data;
+Data required significant transformation to fit the model;
+Confidence intervals are quite wide;
+Data has not been reviewed recently.</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>A 1% Change in the tested input creates a change of between 0.1% and 0.01% in the output(s)</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>Assumptions are usually Red if:
+Unclear/unreliable data source or no data source provided. 
+Based on limited data and methodology not robust. 
+Data is not current. Confidence interval wide/unknown.</t>
+  </si>
+  <si>
+    <t>A 1% Change in the tested input creates &gt;0.1% changein the output(s)</t>
+  </si>
+  <si>
+    <t>An assumption is also sensitive if it changes the direction / commentary of the output.</t>
+  </si>
+  <si>
+    <t>The ethics working group have requested that their ethics log should be linked to as a hyperlink. Use the following link:</t>
+  </si>
+  <si>
+    <t>https://uksa.statisticsauthority.gov.uk/the-authority-board/committees/national-statisticians-advisory-committees-and-panels/national-statisticians-data-ethics-advisory-committee/ethics-self-assessment-tool/</t>
+  </si>
+  <si>
+    <t>When you have completed the ethics log, copy-paste the results into this tab to ensure the log is stored correctly with all other documentation</t>
+  </si>
+  <si>
+    <t>Risk should be understood as the product of quality and sensitivity.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The riskiest assumptions and decisions are those with low evidence quality and high impact on final results. </t>
   </si>
   <si>
     <t>This table indicates a way to calculate risk</t>
   </si>
   <si>
-    <t>The ethics working group have requested that their ethics log should be linked to as a hyperlink. Use the following link:</t>
-  </si>
-  <si>
-    <t>When you have completed the ethics log, copy-paste the results into this tab to ensure the log is stored correctly with all other documentation</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">I agree to communicate the concerns of my analysis team to the commissioner. These concerns can include quality, timeline and feasability concerns. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">I will address </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>the concerns of the analysis team.</t>
-    </r>
+    <t xml:space="preserve">Risk Scoring </t>
+  </si>
+  <si>
+    <t>Med</t>
+  </si>
+  <si>
+    <t>Sensitivity</t>
+  </si>
+  <si>
+    <t>Once risk is calculated, it should be used by teams to ensure that the riskiest assumptions / decisions have the best evidence justifying them.</t>
+  </si>
+  <si>
+    <t>If this is impossible, efforts should be made to reduce the risk by either increasing the quality or reducing the analysis's sensitivity by introducing other independent methodologies.</t>
+  </si>
+  <si>
+    <t>A table with a series of boxes to be filled in by the owning team which sets out basic details about the analysis</t>
+  </si>
+  <si>
+    <t>Most teams will create process maps or model maps during development. These are very helpful to give an overview of the analysis workflow.</t>
+  </si>
+  <si>
+    <t>This table records the assumptions made about the analysis. Assumptions will often be decisions made because there is a need to simplify the situation in the real world to enable it to be analysed or modelled. Wherever possible, such assumptions should have a numerical value and an uncertainty rangel around the value to demonstrate the uncertainty the team has about the assumption. You should also give your assumptions a quality RAG rating. When this is combined with an assessment about sensitivity of the analysis to the assumption, you get an indicative risk score. Use the risk score to inform how resources are allocated to further research and improvement of the assumptions.</t>
+  </si>
+  <si>
+    <t>A at-a-glance guide to quality scoring. If you are not sure about the quality or sensitivity score of an assumption, err on the side of caution and go for lower quality and higher sensitivity.</t>
+  </si>
+  <si>
+    <t>Details</t>
+  </si>
+  <si>
+    <t>This spreadsheet supports analysis development and production by providing a structured template for documentation</t>
   </si>
 </sst>
 </file>
@@ -1746,6 +1746,9 @@
     <xf numFmtId="0" fontId="19" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1817,7 +1820,40 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="2" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1881,47 +1917,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2750,151 +2750,151 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE0E718D-ABA6-478B-BFB8-19647D312746}">
   <dimension ref="B2:D22"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="45"/>
-    <col min="2" max="2" width="15.7109375" style="79" customWidth="1"/>
-    <col min="3" max="3" width="94.28515625" style="52" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="45"/>
+    <col min="2" max="2" width="15.6640625" style="80" customWidth="1"/>
+    <col min="3" max="3" width="94.33203125" style="52" customWidth="1"/>
     <col min="4" max="4" width="39" style="45" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="45"/>
+    <col min="5" max="16384" width="9.109375" style="45"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="98" t="s">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="99" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="99" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="98" t="s">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B4" s="99" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="98" t="s">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B5" s="99" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="98" t="s">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B7" s="56" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="56" t="s">
+      <c r="C7" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="56" t="s">
+      <c r="D7" s="56" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B8" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="56" t="s">
+      <c r="C8" s="79" t="s">
+        <v>200</v>
+      </c>
+      <c r="D8" s="79"/>
+    </row>
+    <row r="9" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B9" s="56" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="56" t="s">
+      <c r="C9" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="78" t="s">
+      <c r="D9" s="79"/>
+    </row>
+    <row r="10" spans="2:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B10" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="78"/>
-    </row>
-    <row r="9" spans="2:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B9" s="56" t="s">
+      <c r="C10" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="78" t="s">
+      <c r="D10" s="79" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="78"/>
-    </row>
-    <row r="10" spans="2:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B10" s="56" t="s">
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B11" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="78" t="s">
+      <c r="C11" s="79" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="78" t="s">
+      <c r="D11" s="79"/>
+    </row>
+    <row r="12" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B12" s="56" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="56" t="s">
+      <c r="C12" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="78" t="s">
+      <c r="D12" s="79"/>
+    </row>
+    <row r="13" spans="2:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="B13" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="78"/>
-    </row>
-    <row r="12" spans="2:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B12" s="56" t="s">
+      <c r="C13" s="81" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="78" t="s">
+      <c r="D13" s="81"/>
+    </row>
+    <row r="14" spans="2:4" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="B14" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="78"/>
-    </row>
-    <row r="13" spans="2:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="B13" s="54" t="s">
+      <c r="C14" s="79" t="s">
+        <v>202</v>
+      </c>
+      <c r="D14" s="79"/>
+    </row>
+    <row r="15" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B15" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="80" t="s">
+      <c r="C15" s="79" t="s">
+        <v>203</v>
+      </c>
+      <c r="D15" s="79"/>
+    </row>
+    <row r="16" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B16" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="80"/>
-    </row>
-    <row r="14" spans="2:4" ht="105" x14ac:dyDescent="0.25">
-      <c r="B14" s="56" t="s">
+      <c r="C16" s="79" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="78" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="78"/>
-    </row>
-    <row r="15" spans="2:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B15" s="56" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="78" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="78"/>
-    </row>
-    <row r="16" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B16" s="56" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="78" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" s="78"/>
-    </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C17" s="79"/>
-      <c r="D17" s="79"/>
-    </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C18" s="79"/>
-      <c r="D18" s="79"/>
-    </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D16" s="79"/>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C17" s="80"/>
+      <c r="D17" s="80"/>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C18" s="80"/>
+      <c r="D18" s="80"/>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D19" s="52"/>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D20" s="52"/>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D21" s="52"/>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D22" s="52"/>
     </row>
   </sheetData>
@@ -2903,6 +2903,42 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{470DF315-86F2-4A76-BD43-D9F1F2DB47B8}">
+  <sheetPr>
+    <tabColor rgb="FF002060"/>
+  </sheetPr>
+  <dimension ref="B2:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B3" s="88" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>191</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{F0927FC3-1838-4B9C-A65A-AFE56E621375}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E243E638-BE3D-4BC2-9B58-98933D2F1E85}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -2910,118 +2946,118 @@
   <dimension ref="B2:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="1"/>
-    <col min="2" max="2" width="42.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="1.5703125" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="1" width="8.6640625" style="1"/>
+    <col min="2" max="2" width="42.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="1.5546875" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B2" s="25" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" ht="48.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="25" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="D6" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D7" s="34"/>
       <c r="E7" s="35"/>
       <c r="F7" s="35"/>
       <c r="G7" s="35"/>
       <c r="H7" s="36" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="I7" s="35"/>
       <c r="J7" s="32"/>
     </row>
-    <row r="8" spans="2:10" ht="6.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" ht="6.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D8" s="37"/>
       <c r="J8" s="26"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="D9" s="38"/>
       <c r="G9" s="29" t="s">
-        <v>162</v>
+        <v>174</v>
       </c>
       <c r="H9" s="29" t="s">
-        <v>166</v>
+        <v>181</v>
       </c>
       <c r="I9" s="29" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="J9" s="26"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="D10" s="38"/>
       <c r="F10" s="28" t="s">
-        <v>164</v>
+        <v>176</v>
       </c>
       <c r="G10" s="33" t="s">
-        <v>164</v>
+        <v>176</v>
       </c>
       <c r="H10" s="33" t="s">
-        <v>164</v>
+        <v>176</v>
       </c>
       <c r="I10" s="33" t="s">
-        <v>174</v>
+        <v>196</v>
       </c>
       <c r="J10" s="26"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="D11" s="39" t="s">
+        <v>197</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>183</v>
+      </c>
+      <c r="G11" s="33" t="s">
+        <v>176</v>
+      </c>
+      <c r="H11" s="33" t="s">
+        <v>196</v>
+      </c>
+      <c r="I11" s="33" t="s">
         <v>175</v>
       </c>
-      <c r="F11" s="28" t="s">
-        <v>167</v>
-      </c>
-      <c r="G11" s="33" t="s">
-        <v>164</v>
-      </c>
-      <c r="H11" s="33" t="s">
-        <v>174</v>
-      </c>
-      <c r="I11" s="33" t="s">
-        <v>163</v>
-      </c>
       <c r="J11" s="26"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="D12" s="38"/>
       <c r="F12" s="28" t="s">
-        <v>163</v>
+        <v>175</v>
       </c>
       <c r="G12" s="33" t="s">
-        <v>174</v>
+        <v>196</v>
       </c>
       <c r="H12" s="33" t="s">
-        <v>163</v>
+        <v>175</v>
       </c>
       <c r="I12" s="33" t="s">
-        <v>163</v>
+        <v>175</v>
       </c>
       <c r="J12" s="26"/>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="D13" s="31"/>
       <c r="E13" s="27"/>
       <c r="F13" s="27"/>
@@ -3030,53 +3066,17 @@
       <c r="I13" s="27"/>
       <c r="J13" s="30"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
-        <v>177</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{470DF315-86F2-4A76-BD43-D9F1F2DB47B8}">
-  <sheetPr>
-    <tabColor rgb="FF002060"/>
-  </sheetPr>
-  <dimension ref="B2:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B3" s="87" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>203</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{F0927FC3-1838-4B9C-A65A-AFE56E621375}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3088,164 +3088,167 @@
   </sheetPr>
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="A1:D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="45"/>
-    <col min="2" max="2" width="23.5703125" style="53" customWidth="1"/>
-    <col min="3" max="3" width="72.85546875" style="45" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="97.42578125" style="45" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="45"/>
+    <col min="1" max="1" width="9.109375" style="45"/>
+    <col min="2" max="2" width="23.5546875" style="53" customWidth="1"/>
+    <col min="3" max="3" width="72.88671875" style="45" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="97.44140625" style="45" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" style="45"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="46" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="46" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="54" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="49"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="55" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="50"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B4" s="55" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="50"/>
+    </row>
+    <row r="5" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B5" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="C5" s="50"/>
+      <c r="D5" s="52" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="54" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B6" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="49"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="55" t="s">
+      <c r="C6" s="48"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="50"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="55" t="s">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B9" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="50"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="55" t="s">
+      <c r="C9" s="49"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B10" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="50"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="56" t="s">
+      <c r="C10" s="47"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B11" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="48"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="46" t="s">
+      <c r="C11" s="51"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="46" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="54" t="s">
+    <row r="14" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B14" s="56" t="s">
         <v>34</v>
-      </c>
-      <c r="C9" s="49"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="56" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="47"/>
-    </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="57" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="51"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="46" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="B14" s="56" t="s">
-        <v>38</v>
       </c>
       <c r="C14" s="48"/>
       <c r="D14" s="58" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B15" s="56" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C15" s="48"/>
       <c r="D15" s="58" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B16" s="56" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C16" s="48"/>
       <c r="D16" s="58" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="46" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="46"/>
       <c r="B19" s="54" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C19" s="50"/>
-      <c r="D19" s="97" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D19" s="98" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="46"/>
       <c r="B20" s="54" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="50"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B21" s="56" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="48"/>
+      <c r="D21" s="98" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="53"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B24" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="50"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="56" t="s">
+      <c r="C24" s="48"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B25" s="54" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="48"/>
-      <c r="D21" s="97" t="s">
+      <c r="C25" s="50"/>
+    </row>
+    <row r="26" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B26" s="56" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="46" t="s">
-        <v>50</v>
-      </c>
-      <c r="B23" s="53"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="56" t="s">
-        <v>51</v>
-      </c>
-      <c r="C24" s="48"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="54" t="s">
-        <v>52</v>
-      </c>
-      <c r="C25" s="50"/>
-    </row>
-    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B26" s="56" t="s">
-        <v>53</v>
       </c>
       <c r="C26" s="48"/>
     </row>
@@ -3265,222 +3268,222 @@
   </sheetPr>
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="45"/>
-    <col min="2" max="2" width="27.140625" style="76" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="45" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" style="45" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" style="45" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" style="52" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="45"/>
-    <col min="8" max="8" width="38.140625" style="45" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="45"/>
+    <col min="1" max="1" width="9.109375" style="45"/>
+    <col min="2" max="2" width="27.109375" style="77" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" style="45" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" style="45" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5546875" style="45" customWidth="1"/>
+    <col min="6" max="6" width="24.88671875" style="52" customWidth="1"/>
+    <col min="7" max="7" width="9.109375" style="45"/>
+    <col min="8" max="8" width="38.109375" style="45" customWidth="1"/>
+    <col min="9" max="16384" width="9.109375" style="45"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="75"/>
-    </row>
-    <row r="2" spans="1:8" s="74" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="73"/>
-      <c r="B2" s="88" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="76"/>
+    </row>
+    <row r="2" spans="1:8" s="75" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="74"/>
+      <c r="B2" s="89" t="s">
+        <v>201</v>
+      </c>
+      <c r="D2" s="74"/>
+      <c r="F2" s="78"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B3" s="89" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B4" s="89" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B5" s="91" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="73"/>
-      <c r="F2" s="77"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="88" t="s">
+    </row>
+    <row r="8" spans="1:8" s="74" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="53" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="88" t="s">
+      <c r="D8" s="74" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="90" t="s">
+      <c r="F8" s="90" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="45" t="s">
+      <c r="H8" s="74" t="s">
         <v>58</v>
       </c>
-      <c r="C7" s="45" t="s">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="46"/>
+      <c r="B10" s="95" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" s="73" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="53" t="s">
+      <c r="F10" s="45"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B11" s="93" t="s">
         <v>60</v>
       </c>
-      <c r="D8" s="73" t="s">
+      <c r="D11" s="45" t="s">
         <v>61</v>
       </c>
-      <c r="F8" s="89" t="s">
+      <c r="F11" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="H8" s="73" t="s">
+      <c r="H11" s="97" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="46"/>
-      <c r="B10" s="94" t="s">
+    <row r="12" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="94" t="s">
         <v>64</v>
       </c>
-      <c r="F10" s="45"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="92" t="s">
+      <c r="D12" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="D11" s="45" t="s">
+      <c r="F12" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="F11" s="45" t="s">
+      <c r="H12" s="96" t="s">
         <v>67</v>
       </c>
-      <c r="H11" s="96" t="s">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B13" s="91"/>
+      <c r="F13" s="45"/>
+      <c r="H13" s="96" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="93" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B14" s="91"/>
+      <c r="F14" s="45"/>
+      <c r="H14" s="96" t="s">
         <v>69</v>
       </c>
-      <c r="D12" s="45" t="s">
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="46"/>
+      <c r="B15" s="95" t="s">
         <v>70</v>
       </c>
-      <c r="F12" s="45" t="s">
+      <c r="F15" s="45"/>
+      <c r="H15" s="96"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B16" s="93" t="s">
         <v>71</v>
       </c>
-      <c r="H12" s="95" t="s">
+      <c r="D16" s="92"/>
+      <c r="F16" s="45"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B17" s="93" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="90"/>
-      <c r="F13" s="45"/>
-      <c r="H13" s="95" t="s">
+      <c r="D17" s="92"/>
+      <c r="F17" s="45"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B18" s="91"/>
+      <c r="D18" s="92"/>
+      <c r="F18" s="45"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B19" s="91"/>
+      <c r="F19" s="45"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B20" s="91"/>
+      <c r="F20" s="45"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="45" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="90"/>
-      <c r="F14" s="45"/>
-      <c r="H14" s="95" t="s">
+      <c r="B21" s="91" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="46"/>
-      <c r="B15" s="94" t="s">
+      <c r="F21" s="45"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B22" s="91" t="s">
         <v>75</v>
       </c>
-      <c r="F15" s="45"/>
-      <c r="H15" s="95"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="92" t="s">
-        <v>76</v>
-      </c>
-      <c r="D16" s="91"/>
-      <c r="F16" s="45"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="92" t="s">
-        <v>77</v>
-      </c>
-      <c r="D17" s="91"/>
-      <c r="F17" s="45"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="90"/>
-      <c r="D18" s="91"/>
-      <c r="F18" s="45"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="90"/>
-      <c r="F19" s="45"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="90"/>
-      <c r="F20" s="45"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="45" t="s">
-        <v>78</v>
-      </c>
-      <c r="B21" s="90" t="s">
-        <v>79</v>
-      </c>
-      <c r="F21" s="45"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="90" t="s">
-        <v>80</v>
-      </c>
       <c r="F22" s="45"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="90"/>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B23" s="91"/>
       <c r="F23" s="45"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="46"/>
-      <c r="B24" s="90"/>
+      <c r="B24" s="91"/>
       <c r="F24" s="45"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="46"/>
-      <c r="B25" s="90"/>
+      <c r="B25" s="91"/>
       <c r="F25" s="45"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="90"/>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B26" s="91"/>
       <c r="F26" s="45"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="90"/>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B27" s="91"/>
       <c r="F27" s="45"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="90"/>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B28" s="91"/>
       <c r="F28" s="45"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="90"/>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B29" s="91"/>
       <c r="F29" s="45"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="90"/>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B30" s="91"/>
       <c r="F30" s="45"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="90"/>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B31" s="91"/>
       <c r="F31" s="45"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="90"/>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B32" s="91"/>
       <c r="F32" s="45"/>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="90"/>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B33" s="91"/>
       <c r="F33" s="45"/>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B34" s="90"/>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B34" s="91"/>
       <c r="F34" s="45"/>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="90"/>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B35" s="91"/>
       <c r="F35" s="45"/>
     </row>
   </sheetData>
@@ -3497,33 +3500,33 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="24.42578125" style="42" customWidth="1"/>
-    <col min="3" max="4" width="16.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="49.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="44.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="58.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="17.140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="16.140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="29.28515625" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="1" width="9.109375" style="1"/>
+    <col min="2" max="2" width="24.44140625" style="42" customWidth="1"/>
+    <col min="3" max="4" width="16.109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="49.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="44.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="58.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17.109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="16.109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="29.33203125" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="H1" s="12"/>
       <c r="I1" s="12"/>
       <c r="J1" s="12"/>
     </row>
-    <row r="2" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="7" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="6"/>
@@ -3534,7 +3537,7 @@
       <c r="J2" s="13"/>
       <c r="K2" s="6"/>
     </row>
-    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -3547,61 +3550,61 @@
       <c r="J3" s="13"/>
       <c r="K3" s="6"/>
     </row>
-    <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
-      <c r="B4" s="99" t="s">
-        <v>82</v>
-      </c>
-      <c r="C4" s="100"/>
-      <c r="D4" s="100"/>
-      <c r="E4" s="100"/>
-      <c r="F4" s="100"/>
-      <c r="G4" s="100"/>
+      <c r="B4" s="111" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="112"/>
+      <c r="D4" s="112"/>
+      <c r="E4" s="112"/>
+      <c r="F4" s="112"/>
+      <c r="G4" s="112"/>
       <c r="H4" s="13"/>
       <c r="I4" s="13"/>
       <c r="J4" s="13"/>
       <c r="K4" s="6"/>
     </row>
-    <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
-      <c r="B5" s="101"/>
-      <c r="C5" s="102"/>
-      <c r="D5" s="102"/>
-      <c r="E5" s="102"/>
-      <c r="F5" s="102"/>
-      <c r="G5" s="102"/>
+      <c r="B5" s="113"/>
+      <c r="C5" s="114"/>
+      <c r="D5" s="114"/>
+      <c r="E5" s="114"/>
+      <c r="F5" s="114"/>
+      <c r="G5" s="114"/>
       <c r="H5" s="13"/>
       <c r="I5" s="13"/>
       <c r="J5" s="13"/>
       <c r="K5" s="6"/>
     </row>
-    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="6"/>
-      <c r="B6" s="101"/>
-      <c r="C6" s="102"/>
-      <c r="D6" s="102"/>
-      <c r="E6" s="102"/>
-      <c r="F6" s="102"/>
-      <c r="G6" s="102"/>
+      <c r="B6" s="113"/>
+      <c r="C6" s="114"/>
+      <c r="D6" s="114"/>
+      <c r="E6" s="114"/>
+      <c r="F6" s="114"/>
+      <c r="G6" s="114"/>
       <c r="H6" s="13"/>
       <c r="I6" s="13"/>
       <c r="J6" s="13"/>
       <c r="K6" s="6"/>
     </row>
-    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
-      <c r="B7" s="103"/>
-      <c r="C7" s="104"/>
-      <c r="D7" s="104"/>
-      <c r="E7" s="104"/>
-      <c r="F7" s="104"/>
-      <c r="G7" s="104"/>
+      <c r="B7" s="115"/>
+      <c r="C7" s="116"/>
+      <c r="D7" s="116"/>
+      <c r="E7" s="116"/>
+      <c r="F7" s="116"/>
+      <c r="G7" s="116"/>
       <c r="H7" s="13"/>
       <c r="I7" s="13"/>
       <c r="J7" s="13"/>
       <c r="K7" s="6"/>
     </row>
-    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -3614,44 +3617,44 @@
       <c r="J8" s="13"/>
       <c r="K8" s="6"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
       <c r="J9" s="12"/>
     </row>
-    <row r="10" spans="1:11" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="39.6" x14ac:dyDescent="0.3">
       <c r="B10" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="G10" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="H10" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="I10" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="J10" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="F10" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="I10" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="J10" s="8" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="17"/>
       <c r="B11" s="43" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
@@ -3663,10 +3666,10 @@
       <c r="J11" s="14"/>
       <c r="K11" s="9"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="9"/>
       <c r="B12" s="43" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
@@ -3678,9 +3681,9 @@
       <c r="J12" s="15"/>
       <c r="K12" s="9"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B13" s="44" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C13" s="41"/>
       <c r="D13" s="41"/>
@@ -3691,17 +3694,17 @@
       <c r="I13" s="41"/>
       <c r="J13" s="41"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="G14" s="18"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="42" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B16" s="43" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
@@ -3712,9 +3715,9 @@
       <c r="I16" s="15"/>
       <c r="J16" s="14"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B17" s="43" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C17" s="11"/>
       <c r="D17" s="11"/>
@@ -3725,9 +3728,9 @@
       <c r="I17" s="15"/>
       <c r="J17" s="15"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B18" s="44" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C18" s="41"/>
       <c r="D18" s="41"/>
@@ -3759,127 +3762,127 @@
   </sheetPr>
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection sqref="A1:N18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" style="62" customWidth="1"/>
-    <col min="2" max="2" width="103.28515625" style="62" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="62" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.140625" style="62"/>
+    <col min="1" max="1" width="18.88671875" style="62" customWidth="1"/>
+    <col min="2" max="2" width="103.33203125" style="62" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" style="62" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.109375" style="62"/>
     <col min="6" max="6" width="30" style="62" customWidth="1"/>
-    <col min="7" max="7" width="71.5703125" style="59" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" style="62" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="9.140625" style="62"/>
+    <col min="7" max="7" width="71.5546875" style="59" customWidth="1"/>
+    <col min="8" max="8" width="15.44140625" style="62" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.109375" style="62"/>
     <col min="11" max="11" width="30" style="62" customWidth="1"/>
-    <col min="12" max="12" width="97.5703125" style="62" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" style="62" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="62"/>
+    <col min="12" max="12" width="97.5546875" style="62" customWidth="1"/>
+    <col min="13" max="13" width="14.44140625" style="62" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.109375" style="62"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="61" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="63" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="61"/>
+    </row>
+    <row r="4" spans="1:14" ht="69" x14ac:dyDescent="0.25">
+      <c r="A4" s="100" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" s="102" t="s">
+        <v>94</v>
+      </c>
+      <c r="F4" s="101" t="s">
+        <v>95</v>
+      </c>
+      <c r="G4" s="103" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="61"/>
-    </row>
-    <row r="4" spans="1:14" ht="87.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="121" t="s">
+      <c r="H4" s="73"/>
+      <c r="I4" s="73"/>
+      <c r="J4" s="73"/>
+      <c r="K4" s="64" t="s">
         <v>97</v>
       </c>
-      <c r="B4" s="123" t="s">
-        <v>179</v>
-      </c>
-      <c r="F4" s="122" t="s">
+      <c r="L4" s="103" t="s">
         <v>98</v>
       </c>
-      <c r="G4" s="124" t="s">
-        <v>180</v>
-      </c>
-      <c r="H4" s="72"/>
-      <c r="I4" s="72"/>
-      <c r="J4" s="72"/>
-      <c r="K4" s="64" t="s">
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="61"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="61"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="72" t="s">
         <v>99</v>
       </c>
-      <c r="L4" s="124" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="61"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="61"/>
-    </row>
-    <row r="7" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="71" t="s">
+      <c r="F7" s="72" t="s">
         <v>100</v>
-      </c>
-      <c r="F7" s="71" t="s">
-        <v>101</v>
       </c>
       <c r="G7" s="66"/>
       <c r="K7" s="65" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" s="65" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="67" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" s="65" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B8" s="67" t="s">
+      <c r="C8" s="67" t="s">
         <v>103</v>
       </c>
-      <c r="C8" s="67" t="s">
+      <c r="D8" s="67" t="s">
         <v>104</v>
       </c>
-      <c r="D8" s="67" t="s">
+      <c r="G8" s="67" t="s">
+        <v>102</v>
+      </c>
+      <c r="H8" s="67" t="s">
+        <v>103</v>
+      </c>
+      <c r="I8" s="67" t="s">
+        <v>104</v>
+      </c>
+      <c r="L8" s="67" t="s">
+        <v>102</v>
+      </c>
+      <c r="M8" s="67" t="s">
+        <v>103</v>
+      </c>
+      <c r="N8" s="67" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="B9" s="60" t="s">
         <v>105</v>
-      </c>
-      <c r="G8" s="67" t="s">
-        <v>103</v>
-      </c>
-      <c r="H8" s="67" t="s">
-        <v>104</v>
-      </c>
-      <c r="I8" s="67" t="s">
-        <v>105</v>
-      </c>
-      <c r="L8" s="67" t="s">
-        <v>103</v>
-      </c>
-      <c r="M8" s="67" t="s">
-        <v>104</v>
-      </c>
-      <c r="N8" s="67" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="B9" s="60" t="s">
-        <v>106</v>
       </c>
       <c r="C9" s="69"/>
       <c r="D9" s="69"/>
-      <c r="G9" s="125" t="s">
-        <v>107</v>
+      <c r="G9" s="104" t="s">
+        <v>106</v>
       </c>
       <c r="H9" s="69"/>
       <c r="I9" s="69"/>
-      <c r="L9" s="125" t="s">
-        <v>185</v>
+      <c r="L9" s="104" t="s">
+        <v>107</v>
       </c>
       <c r="M9" s="69"/>
       <c r="N9" s="69"/>
     </row>
-    <row r="10" spans="1:14" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" ht="41.4" x14ac:dyDescent="0.25">
       <c r="B10" s="60" t="s">
         <v>108</v>
       </c>
@@ -3890,71 +3893,71 @@
       </c>
       <c r="H10" s="69"/>
       <c r="I10" s="69"/>
-      <c r="L10" s="125" t="s">
-        <v>186</v>
+      <c r="L10" s="104" t="s">
+        <v>110</v>
       </c>
       <c r="M10" s="69"/>
       <c r="N10" s="69"/>
     </row>
-    <row r="11" spans="1:14" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B11" s="60" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C11" s="69"/>
       <c r="D11" s="69"/>
-      <c r="G11" s="125" t="s">
-        <v>181</v>
+      <c r="G11" s="104" t="s">
+        <v>112</v>
       </c>
       <c r="H11" s="69"/>
       <c r="I11" s="69"/>
       <c r="L11" s="70" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="M11" s="69"/>
       <c r="N11" s="69"/>
     </row>
-    <row r="12" spans="1:14" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B12" s="60" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C12" s="69"/>
       <c r="D12" s="69"/>
-      <c r="G12" s="125" t="s">
-        <v>182</v>
+      <c r="G12" s="104" t="s">
+        <v>115</v>
       </c>
       <c r="H12" s="69"/>
       <c r="I12" s="69"/>
-      <c r="L12" s="125" t="s">
-        <v>189</v>
+      <c r="L12" s="104" t="s">
+        <v>116</v>
       </c>
       <c r="M12" s="69"/>
       <c r="N12" s="69"/>
     </row>
-    <row r="13" spans="1:14" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" ht="41.4" x14ac:dyDescent="0.25">
       <c r="B13" s="60" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="C13" s="69"/>
       <c r="D13" s="69"/>
-      <c r="G13" s="126" t="s">
-        <v>183</v>
+      <c r="G13" s="105" t="s">
+        <v>118</v>
       </c>
       <c r="H13" s="69"/>
       <c r="I13" s="69"/>
       <c r="L13" s="60" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="M13" s="69"/>
       <c r="N13" s="69"/>
     </row>
-    <row r="14" spans="1:14" ht="43.5" x14ac:dyDescent="0.25">
-      <c r="B14" s="133" t="s">
-        <v>204</v>
+    <row r="14" spans="1:14" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="B14" s="71" t="s">
+        <v>120</v>
       </c>
       <c r="C14" s="69"/>
       <c r="D14" s="69"/>
-      <c r="G14" s="126" t="s">
-        <v>184</v>
+      <c r="G14" s="105" t="s">
+        <v>121</v>
       </c>
       <c r="H14" s="69"/>
       <c r="I14" s="69"/>
@@ -3962,48 +3965,48 @@
       <c r="M14" s="69"/>
       <c r="N14" s="69"/>
     </row>
-    <row r="16" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="65" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="F16" s="65" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="K16" s="65" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="17" spans="7:14" ht="15" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="17" spans="7:14" x14ac:dyDescent="0.25">
       <c r="G17" s="68" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="H17" s="67" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="I17" s="67" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="L17" s="67" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="M17" s="67" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="N17" s="67" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="18" spans="7:14" ht="100.5" x14ac:dyDescent="0.2">
-      <c r="G18" s="127" t="s">
-        <v>187</v>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="18" spans="7:14" ht="82.8" x14ac:dyDescent="0.25">
+      <c r="G18" s="106" t="s">
+        <v>128</v>
       </c>
       <c r="H18" s="69"/>
       <c r="I18" s="69"/>
       <c r="J18" s="62" t="s">
-        <v>121</v>
-      </c>
-      <c r="L18" s="127" t="s">
-        <v>188</v>
+        <v>129</v>
+      </c>
+      <c r="L18" s="106" t="s">
+        <v>130</v>
       </c>
       <c r="M18" s="69"/>
       <c r="N18" s="69"/>
@@ -4023,217 +4026,217 @@
   <dimension ref="A2:H36"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
+      <pane ySplit="10" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="65.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="70.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="65.5546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="70.44140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="42" style="1" customWidth="1"/>
-    <col min="7" max="7" width="29.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="28.42578125" style="12" customWidth="1"/>
+    <col min="7" max="7" width="29.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="28.44140625" style="12" customWidth="1"/>
     <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" s="6" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" s="6" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="D2" s="7" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="F2" s="24" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="H2" s="13"/>
     </row>
-    <row r="3" spans="1:8" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H3" s="13"/>
     </row>
-    <row r="4" spans="1:8" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="99" t="s">
-        <v>124</v>
-      </c>
-      <c r="C4" s="105"/>
-      <c r="D4" s="100"/>
-      <c r="E4" s="100"/>
-      <c r="F4" s="100"/>
-      <c r="G4" s="106"/>
+    <row r="4" spans="1:8" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B4" s="111" t="s">
+        <v>133</v>
+      </c>
+      <c r="C4" s="117"/>
+      <c r="D4" s="112"/>
+      <c r="E4" s="112"/>
+      <c r="F4" s="112"/>
+      <c r="G4" s="118"/>
       <c r="H4" s="13"/>
     </row>
-    <row r="5" spans="1:8" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="101"/>
-      <c r="C5" s="102"/>
-      <c r="D5" s="102"/>
-      <c r="E5" s="102"/>
-      <c r="F5" s="102"/>
-      <c r="G5" s="107"/>
+    <row r="5" spans="1:8" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B5" s="113"/>
+      <c r="C5" s="114"/>
+      <c r="D5" s="114"/>
+      <c r="E5" s="114"/>
+      <c r="F5" s="114"/>
+      <c r="G5" s="119"/>
       <c r="H5" s="13"/>
     </row>
-    <row r="6" spans="1:8" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="101"/>
-      <c r="C6" s="102"/>
-      <c r="D6" s="102"/>
-      <c r="E6" s="102"/>
-      <c r="F6" s="102"/>
-      <c r="G6" s="107"/>
+    <row r="6" spans="1:8" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B6" s="113"/>
+      <c r="C6" s="114"/>
+      <c r="D6" s="114"/>
+      <c r="E6" s="114"/>
+      <c r="F6" s="114"/>
+      <c r="G6" s="119"/>
       <c r="H6" s="13"/>
     </row>
-    <row r="7" spans="1:8" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="103"/>
-      <c r="C7" s="104"/>
-      <c r="D7" s="104"/>
-      <c r="E7" s="104"/>
-      <c r="F7" s="104"/>
-      <c r="G7" s="108"/>
+    <row r="7" spans="1:8" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B7" s="115"/>
+      <c r="C7" s="116"/>
+      <c r="D7" s="116"/>
+      <c r="E7" s="116"/>
+      <c r="F7" s="116"/>
+      <c r="G7" s="120"/>
       <c r="H7" s="13"/>
     </row>
-    <row r="8" spans="1:8" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B8" s="16"/>
       <c r="C8" s="16"/>
       <c r="H8" s="13"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B10" s="8" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" s="9" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="9" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="17"/>
       <c r="B11" s="10">
         <v>1</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="G11" s="23" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="H11" s="14"/>
     </row>
-    <row r="12" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D12" s="18"/>
       <c r="E12" s="18"/>
       <c r="F12" s="18"/>
       <c r="H12" s="19"/>
     </row>
-    <row r="13" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D13" s="18"/>
       <c r="E13" s="18"/>
       <c r="F13" s="18"/>
       <c r="H13" s="19"/>
     </row>
-    <row r="14" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D14" s="18"/>
       <c r="E14" s="18"/>
       <c r="F14" s="18"/>
       <c r="H14" s="19"/>
     </row>
-    <row r="15" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D15" s="18"/>
       <c r="E15" s="18"/>
       <c r="F15" s="18"/>
       <c r="H15" s="19"/>
     </row>
-    <row r="16" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D16" s="18"/>
       <c r="E16" s="18"/>
       <c r="F16" s="18"/>
       <c r="H16" s="19"/>
     </row>
-    <row r="17" spans="4:8" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:8" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D17" s="18"/>
       <c r="E17" s="18"/>
       <c r="F17" s="18"/>
       <c r="H17" s="19"/>
     </row>
-    <row r="18" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D18" s="18"/>
       <c r="E18" s="18"/>
       <c r="F18" s="18"/>
       <c r="H18" s="19"/>
     </row>
-    <row r="19" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="H19" s="20"/>
     </row>
-    <row r="20" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="H20" s="20"/>
     </row>
-    <row r="21" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="H21" s="20"/>
     </row>
-    <row r="22" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="H22" s="20"/>
     </row>
-    <row r="23" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="H23" s="20"/>
     </row>
-    <row r="24" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="H24" s="20"/>
     </row>
-    <row r="25" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="H25" s="20"/>
     </row>
-    <row r="26" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="H26" s="20"/>
     </row>
-    <row r="27" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="H27" s="20"/>
     </row>
-    <row r="28" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="H28" s="20"/>
     </row>
-    <row r="29" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="H29" s="20"/>
     </row>
-    <row r="30" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="H30" s="20"/>
     </row>
-    <row r="31" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="H31" s="20"/>
     </row>
-    <row r="32" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="H32" s="20"/>
     </row>
-    <row r="33" spans="8:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="8:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="H33" s="20"/>
     </row>
-    <row r="34" spans="8:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="8:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="H34" s="20"/>
     </row>
-    <row r="35" spans="8:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="8:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="H35" s="20"/>
     </row>
-    <row r="36" spans="8:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="8:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="H36" s="20"/>
     </row>
   </sheetData>
@@ -4260,38 +4263,38 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="8.7109375" style="1"/>
-    <col min="3" max="4" width="16.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="49.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="44.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="58.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="30.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="17.140625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="16.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="29.28515625" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="2" width="8.6640625" style="1"/>
+    <col min="3" max="4" width="16.109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="49.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="44.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="58.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="30.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="17.109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="16.109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="29.33203125" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="J1" s="12"/>
       <c r="K1" s="12"/>
       <c r="L1" s="12"/>
     </row>
-    <row r="2" spans="1:13" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="7" t="s">
-        <v>192</v>
+        <v>146</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="H2" s="24" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="I2" s="24"/>
       <c r="J2" s="13"/>
@@ -4299,7 +4302,7 @@
       <c r="L2" s="13"/>
       <c r="M2" s="6"/>
     </row>
-    <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -4314,69 +4317,69 @@
       <c r="L3" s="13"/>
       <c r="M3" s="6"/>
     </row>
-    <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
-      <c r="B4" s="109" t="s">
-        <v>193</v>
-      </c>
-      <c r="C4" s="110"/>
-      <c r="D4" s="110"/>
-      <c r="E4" s="110"/>
-      <c r="F4" s="110"/>
-      <c r="G4" s="110"/>
-      <c r="H4" s="111"/>
+      <c r="B4" s="121" t="s">
+        <v>147</v>
+      </c>
+      <c r="C4" s="122"/>
+      <c r="D4" s="122"/>
+      <c r="E4" s="122"/>
+      <c r="F4" s="122"/>
+      <c r="G4" s="122"/>
+      <c r="H4" s="123"/>
       <c r="I4" s="40"/>
       <c r="J4" s="13"/>
       <c r="K4" s="13"/>
       <c r="L4" s="13"/>
       <c r="M4" s="6"/>
     </row>
-    <row r="5" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
-      <c r="B5" s="112"/>
-      <c r="C5" s="102"/>
-      <c r="D5" s="102"/>
-      <c r="E5" s="102"/>
-      <c r="F5" s="102"/>
-      <c r="G5" s="102"/>
-      <c r="H5" s="113"/>
+      <c r="B5" s="124"/>
+      <c r="C5" s="114"/>
+      <c r="D5" s="114"/>
+      <c r="E5" s="114"/>
+      <c r="F5" s="114"/>
+      <c r="G5" s="114"/>
+      <c r="H5" s="125"/>
       <c r="I5" s="40"/>
       <c r="J5" s="13"/>
       <c r="K5" s="13"/>
       <c r="L5" s="13"/>
       <c r="M5" s="6"/>
     </row>
-    <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="6"/>
-      <c r="B6" s="112"/>
-      <c r="C6" s="102"/>
-      <c r="D6" s="102"/>
-      <c r="E6" s="102"/>
-      <c r="F6" s="102"/>
-      <c r="G6" s="102"/>
-      <c r="H6" s="113"/>
+      <c r="B6" s="124"/>
+      <c r="C6" s="114"/>
+      <c r="D6" s="114"/>
+      <c r="E6" s="114"/>
+      <c r="F6" s="114"/>
+      <c r="G6" s="114"/>
+      <c r="H6" s="125"/>
       <c r="I6" s="40"/>
       <c r="J6" s="13"/>
       <c r="K6" s="13"/>
       <c r="L6" s="13"/>
       <c r="M6" s="6"/>
     </row>
-    <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
-      <c r="B7" s="114"/>
-      <c r="C7" s="115"/>
-      <c r="D7" s="115"/>
-      <c r="E7" s="115"/>
-      <c r="F7" s="115"/>
-      <c r="G7" s="115"/>
-      <c r="H7" s="116"/>
+      <c r="B7" s="126"/>
+      <c r="C7" s="127"/>
+      <c r="D7" s="127"/>
+      <c r="E7" s="127"/>
+      <c r="F7" s="127"/>
+      <c r="G7" s="127"/>
+      <c r="H7" s="128"/>
       <c r="I7" s="40"/>
       <c r="J7" s="13"/>
       <c r="K7" s="13"/>
       <c r="L7" s="13"/>
       <c r="M7" s="6"/>
     </row>
-    <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="6"/>
       <c r="B8" s="16"/>
       <c r="C8" s="6"/>
@@ -4391,47 +4394,47 @@
       <c r="L8" s="13"/>
       <c r="M8" s="6"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="J9" s="12"/>
       <c r="K9" s="12"/>
       <c r="L9" s="12"/>
     </row>
-    <row r="10" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="26.4" x14ac:dyDescent="0.3">
       <c r="B10" s="8" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>139</v>
+        <v>150</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>144</v>
+        <v>155</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>145</v>
+        <v>156</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="17"/>
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
@@ -4446,7 +4449,7 @@
       <c r="L11" s="14"/>
       <c r="M11" s="9"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="9"/>
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
@@ -4461,7 +4464,7 @@
       <c r="L12" s="15"/>
       <c r="M12" s="9"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B13" s="41"/>
       <c r="C13" s="41"/>
       <c r="D13" s="41"/>
@@ -4474,7 +4477,7 @@
       <c r="K13" s="41"/>
       <c r="L13" s="41"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B14" s="41"/>
       <c r="C14" s="41"/>
       <c r="D14" s="41"/>
@@ -4487,7 +4490,7 @@
       <c r="K14" s="41"/>
       <c r="L14" s="41"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B15" s="41"/>
       <c r="C15" s="41"/>
       <c r="D15" s="41"/>
@@ -4500,7 +4503,7 @@
       <c r="K15" s="41"/>
       <c r="L15" s="41"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B16" s="41"/>
       <c r="C16" s="41"/>
       <c r="D16" s="41"/>
@@ -4513,7 +4516,7 @@
       <c r="K16" s="41"/>
       <c r="L16" s="41"/>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B17" s="41"/>
       <c r="C17" s="41"/>
       <c r="D17" s="41"/>
@@ -4526,7 +4529,7 @@
       <c r="K17" s="41"/>
       <c r="L17" s="41"/>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B18" s="41"/>
       <c r="C18" s="41"/>
       <c r="D18" s="41"/>
@@ -4539,7 +4542,7 @@
       <c r="K18" s="41"/>
       <c r="L18" s="41"/>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B19" s="41"/>
       <c r="C19" s="41"/>
       <c r="D19" s="41"/>
@@ -4552,7 +4555,7 @@
       <c r="K19" s="41"/>
       <c r="L19" s="41"/>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B20" s="41"/>
       <c r="C20" s="41"/>
       <c r="D20" s="41"/>
@@ -4565,7 +4568,7 @@
       <c r="K20" s="41"/>
       <c r="L20" s="41"/>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B21" s="41"/>
       <c r="C21" s="41"/>
       <c r="D21" s="41"/>
@@ -4578,7 +4581,7 @@
       <c r="K21" s="41"/>
       <c r="L21" s="41"/>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B22" s="41"/>
       <c r="C22" s="41"/>
       <c r="D22" s="41"/>
@@ -4618,33 +4621,33 @@
       <selection pane="bottomLeft" activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="65.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="33.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="32.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="33.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="53.140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="38.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="65.5546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="33.88671875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="32.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="33.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="53.109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="38.6640625" style="1" customWidth="1"/>
     <col min="10" max="10" width="26" style="1" customWidth="1"/>
     <col min="11" max="11" width="15" style="12" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" style="12" customWidth="1"/>
-    <col min="13" max="16" width="17.28515625" style="12" customWidth="1"/>
+    <col min="12" max="12" width="12.88671875" style="12" customWidth="1"/>
+    <col min="13" max="16" width="17.33203125" style="12" customWidth="1"/>
     <col min="17" max="17" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:19" s="6" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" s="6" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="D2" s="7" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
       <c r="I2" s="24" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="K2" s="13"/>
       <c r="L2" s="13"/>
@@ -4653,7 +4656,7 @@
       <c r="O2" s="13"/>
       <c r="P2" s="13"/>
     </row>
-    <row r="3" spans="1:19" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
       <c r="M3" s="13"/>
@@ -4661,18 +4664,18 @@
       <c r="O3" s="13"/>
       <c r="P3" s="13"/>
     </row>
-    <row r="4" spans="1:19" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="99" t="s">
-        <v>194</v>
-      </c>
-      <c r="C4" s="105"/>
-      <c r="D4" s="100"/>
-      <c r="E4" s="100"/>
-      <c r="F4" s="100"/>
-      <c r="G4" s="100"/>
-      <c r="H4" s="100"/>
-      <c r="I4" s="100"/>
-      <c r="J4" s="106"/>
+    <row r="4" spans="1:19" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B4" s="111" t="s">
+        <v>158</v>
+      </c>
+      <c r="C4" s="117"/>
+      <c r="D4" s="112"/>
+      <c r="E4" s="112"/>
+      <c r="F4" s="112"/>
+      <c r="G4" s="112"/>
+      <c r="H4" s="112"/>
+      <c r="I4" s="112"/>
+      <c r="J4" s="118"/>
       <c r="K4" s="13"/>
       <c r="L4" s="13"/>
       <c r="M4" s="13"/>
@@ -4680,16 +4683,16 @@
       <c r="O4" s="13"/>
       <c r="P4" s="13"/>
     </row>
-    <row r="5" spans="1:19" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="101"/>
-      <c r="C5" s="102"/>
-      <c r="D5" s="102"/>
-      <c r="E5" s="102"/>
-      <c r="F5" s="102"/>
-      <c r="G5" s="102"/>
-      <c r="H5" s="102"/>
-      <c r="I5" s="102"/>
-      <c r="J5" s="107"/>
+    <row r="5" spans="1:19" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B5" s="113"/>
+      <c r="C5" s="114"/>
+      <c r="D5" s="114"/>
+      <c r="E5" s="114"/>
+      <c r="F5" s="114"/>
+      <c r="G5" s="114"/>
+      <c r="H5" s="114"/>
+      <c r="I5" s="114"/>
+      <c r="J5" s="119"/>
       <c r="K5" s="13"/>
       <c r="L5" s="13"/>
       <c r="M5" s="13"/>
@@ -4697,16 +4700,16 @@
       <c r="O5" s="13"/>
       <c r="P5" s="13"/>
     </row>
-    <row r="6" spans="1:19" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="101"/>
-      <c r="C6" s="102"/>
-      <c r="D6" s="102"/>
-      <c r="E6" s="102"/>
-      <c r="F6" s="102"/>
-      <c r="G6" s="102"/>
-      <c r="H6" s="102"/>
-      <c r="I6" s="102"/>
-      <c r="J6" s="107"/>
+    <row r="6" spans="1:19" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B6" s="113"/>
+      <c r="C6" s="114"/>
+      <c r="D6" s="114"/>
+      <c r="E6" s="114"/>
+      <c r="F6" s="114"/>
+      <c r="G6" s="114"/>
+      <c r="H6" s="114"/>
+      <c r="I6" s="114"/>
+      <c r="J6" s="119"/>
       <c r="K6" s="13"/>
       <c r="L6" s="13"/>
       <c r="M6" s="13"/>
@@ -4714,16 +4717,16 @@
       <c r="O6" s="13"/>
       <c r="P6" s="13"/>
     </row>
-    <row r="7" spans="1:19" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="103"/>
-      <c r="C7" s="104"/>
-      <c r="D7" s="104"/>
-      <c r="E7" s="104"/>
-      <c r="F7" s="104"/>
-      <c r="G7" s="104"/>
-      <c r="H7" s="104"/>
-      <c r="I7" s="104"/>
-      <c r="J7" s="108"/>
+    <row r="7" spans="1:19" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B7" s="115"/>
+      <c r="C7" s="116"/>
+      <c r="D7" s="116"/>
+      <c r="E7" s="116"/>
+      <c r="F7" s="116"/>
+      <c r="G7" s="116"/>
+      <c r="H7" s="116"/>
+      <c r="I7" s="116"/>
+      <c r="J7" s="120"/>
       <c r="K7" s="13"/>
       <c r="L7" s="13"/>
       <c r="M7" s="13"/>
@@ -4731,7 +4734,7 @@
       <c r="O7" s="13"/>
       <c r="P7" s="13"/>
     </row>
-    <row r="8" spans="1:19" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B8" s="16"/>
       <c r="C8" s="16"/>
       <c r="K8" s="13"/>
@@ -4741,63 +4744,63 @@
       <c r="O8" s="13"/>
       <c r="P8" s="13"/>
     </row>
-    <row r="10" spans="1:19" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" ht="39.6" x14ac:dyDescent="0.3">
       <c r="B10" s="8" t="s">
-        <v>147</v>
+        <v>159</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>149</v>
+        <v>161</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>150</v>
+        <v>162</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>151</v>
+        <v>163</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>152</v>
+        <v>164</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>153</v>
+        <v>165</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>154</v>
+        <v>166</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>155</v>
+        <v>167</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>156</v>
+        <v>168</v>
       </c>
       <c r="M10" s="8" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="N10" s="8" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="O10" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="P10" s="83" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q10" s="85" t="s">
-        <v>159</v>
-      </c>
-      <c r="R10" s="85" t="s">
-        <v>160</v>
-      </c>
-      <c r="S10" s="85" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" s="9" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+      <c r="P10" s="84" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q10" s="86" t="s">
+        <v>171</v>
+      </c>
+      <c r="R10" s="86" t="s">
+        <v>172</v>
+      </c>
+      <c r="S10" s="86" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" s="9" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="17"/>
       <c r="B11" s="10">
         <v>1</v>
@@ -4805,8 +4808,8 @@
       <c r="C11" s="10"/>
       <c r="D11" s="11"/>
       <c r="E11" s="11"/>
-      <c r="F11" s="81"/>
-      <c r="G11" s="81"/>
+      <c r="F11" s="82"/>
+      <c r="G11" s="82"/>
       <c r="H11" s="11"/>
       <c r="I11" s="11"/>
       <c r="J11" s="23"/>
@@ -4816,17 +4819,17 @@
       <c r="N11" s="14"/>
       <c r="O11" s="14"/>
       <c r="P11" s="14"/>
-      <c r="Q11" s="84" t="s">
-        <v>162</v>
-      </c>
-      <c r="R11" s="86" t="s">
-        <v>163</v>
-      </c>
-      <c r="S11" s="86" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q11" s="85" t="s">
+        <v>174</v>
+      </c>
+      <c r="R11" s="87" t="s">
+        <v>175</v>
+      </c>
+      <c r="S11" s="87" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="D12" s="18"/>
       <c r="E12" s="18"/>
       <c r="F12" s="18"/>
@@ -4841,7 +4844,7 @@
       <c r="P12" s="20"/>
       <c r="Q12" s="22"/>
     </row>
-    <row r="13" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="D13" s="18"/>
       <c r="E13" s="18"/>
       <c r="F13" s="18"/>
@@ -4856,7 +4859,7 @@
       <c r="P13" s="20"/>
       <c r="Q13" s="22"/>
     </row>
-    <row r="14" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="D14" s="18"/>
       <c r="E14" s="18"/>
       <c r="F14" s="18"/>
@@ -4871,7 +4874,7 @@
       <c r="P14" s="20"/>
       <c r="Q14" s="21"/>
     </row>
-    <row r="15" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="D15" s="18"/>
       <c r="E15" s="18"/>
       <c r="F15" s="18"/>
@@ -4886,7 +4889,7 @@
       <c r="P15" s="20"/>
       <c r="Q15" s="21"/>
     </row>
-    <row r="16" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="D16" s="18"/>
       <c r="E16" s="18"/>
       <c r="F16" s="18"/>
@@ -4901,7 +4904,7 @@
       <c r="P16" s="20"/>
       <c r="Q16" s="21"/>
     </row>
-    <row r="17" spans="4:17" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:17" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D17" s="18"/>
       <c r="E17" s="18"/>
       <c r="F17" s="18"/>
@@ -4916,7 +4919,7 @@
       <c r="P17" s="20"/>
       <c r="Q17" s="21"/>
     </row>
-    <row r="18" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:17" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="D18" s="18"/>
       <c r="E18" s="18"/>
       <c r="F18" s="18"/>
@@ -4931,7 +4934,7 @@
       <c r="P18" s="20"/>
       <c r="Q18" s="21"/>
     </row>
-    <row r="19" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:17" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="K19" s="20"/>
       <c r="L19" s="20"/>
       <c r="M19" s="20"/>
@@ -4940,7 +4943,7 @@
       <c r="P19" s="20"/>
       <c r="Q19" s="22"/>
     </row>
-    <row r="20" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:17" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="K20" s="20"/>
       <c r="L20" s="20"/>
       <c r="M20" s="20"/>
@@ -4949,7 +4952,7 @@
       <c r="P20" s="20"/>
       <c r="Q20" s="22"/>
     </row>
-    <row r="21" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:17" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="K21" s="20"/>
       <c r="L21" s="20"/>
       <c r="M21" s="20"/>
@@ -4958,7 +4961,7 @@
       <c r="P21" s="20"/>
       <c r="Q21" s="22"/>
     </row>
-    <row r="22" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:17" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="K22" s="20"/>
       <c r="L22" s="20"/>
       <c r="M22" s="20"/>
@@ -4967,7 +4970,7 @@
       <c r="P22" s="20"/>
       <c r="Q22" s="22"/>
     </row>
-    <row r="23" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:17" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="K23" s="20"/>
       <c r="L23" s="20"/>
       <c r="M23" s="20"/>
@@ -4976,7 +4979,7 @@
       <c r="P23" s="20"/>
       <c r="Q23" s="22"/>
     </row>
-    <row r="24" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:17" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="K24" s="20"/>
       <c r="L24" s="20"/>
       <c r="M24" s="20"/>
@@ -4985,7 +4988,7 @@
       <c r="P24" s="20"/>
       <c r="Q24" s="22"/>
     </row>
-    <row r="25" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:17" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="K25" s="20"/>
       <c r="L25" s="20"/>
       <c r="M25" s="20"/>
@@ -4994,7 +4997,7 @@
       <c r="P25" s="20"/>
       <c r="Q25" s="22"/>
     </row>
-    <row r="26" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:17" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="K26" s="20"/>
       <c r="L26" s="20"/>
       <c r="M26" s="20"/>
@@ -5003,7 +5006,7 @@
       <c r="P26" s="20"/>
       <c r="Q26" s="22"/>
     </row>
-    <row r="27" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:17" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="K27" s="20"/>
       <c r="L27" s="20"/>
       <c r="M27" s="20"/>
@@ -5012,7 +5015,7 @@
       <c r="P27" s="20"/>
       <c r="Q27" s="22"/>
     </row>
-    <row r="28" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:17" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="K28" s="20"/>
       <c r="L28" s="20"/>
       <c r="M28" s="20"/>
@@ -5021,7 +5024,7 @@
       <c r="P28" s="20"/>
       <c r="Q28" s="22"/>
     </row>
-    <row r="29" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:17" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="K29" s="20"/>
       <c r="L29" s="20"/>
       <c r="M29" s="20"/>
@@ -5030,7 +5033,7 @@
       <c r="P29" s="20"/>
       <c r="Q29" s="22"/>
     </row>
-    <row r="30" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:17" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="K30" s="20"/>
       <c r="L30" s="20"/>
       <c r="M30" s="20"/>
@@ -5039,7 +5042,7 @@
       <c r="P30" s="20"/>
       <c r="Q30" s="22"/>
     </row>
-    <row r="31" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:17" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="K31" s="20"/>
       <c r="L31" s="20"/>
       <c r="M31" s="20"/>
@@ -5048,7 +5051,7 @@
       <c r="P31" s="20"/>
       <c r="Q31" s="22"/>
     </row>
-    <row r="32" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:17" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="K32" s="20"/>
       <c r="L32" s="20"/>
       <c r="M32" s="20"/>
@@ -5057,7 +5060,7 @@
       <c r="P32" s="20"/>
       <c r="Q32" s="22"/>
     </row>
-    <row r="33" spans="11:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="11:17" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="K33" s="20"/>
       <c r="L33" s="20"/>
       <c r="M33" s="20"/>
@@ -5066,7 +5069,7 @@
       <c r="P33" s="20"/>
       <c r="Q33" s="22"/>
     </row>
-    <row r="34" spans="11:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="11:17" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="K34" s="20"/>
       <c r="L34" s="20"/>
       <c r="M34" s="20"/>
@@ -5075,7 +5078,7 @@
       <c r="P34" s="20"/>
       <c r="Q34" s="22"/>
     </row>
-    <row r="35" spans="11:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="11:17" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="K35" s="20"/>
       <c r="L35" s="20"/>
       <c r="M35" s="20"/>
@@ -5084,7 +5087,7 @@
       <c r="P35" s="20"/>
       <c r="Q35" s="22"/>
     </row>
-    <row r="36" spans="11:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="11:17" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="K36" s="20"/>
       <c r="L36" s="20"/>
       <c r="M36" s="20"/>
@@ -5133,94 +5136,94 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
     <col min="2" max="2" width="30" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="37.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="37.109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="1"/>
-    <col min="6" max="6" width="26.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="26.33203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="9" style="1"/>
-    <col min="8" max="8" width="42.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="42.88671875" style="1" customWidth="1"/>
     <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:8" ht="138.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="138.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
-      <c r="B2" s="117" t="s">
-        <v>200</v>
-      </c>
-      <c r="C2" s="130" t="s">
-        <v>162</v>
+      <c r="B2" s="129" t="s">
+        <v>177</v>
+      </c>
+      <c r="C2" s="109" t="s">
+        <v>174</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>195</v>
+        <v>178</v>
       </c>
       <c r="F2" s="132" t="s">
-        <v>199</v>
-      </c>
-      <c r="G2" s="131" t="s">
-        <v>164</v>
-      </c>
-      <c r="H2" s="82" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="144.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+      <c r="G2" s="110" t="s">
+        <v>176</v>
+      </c>
+      <c r="H2" s="83" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="144.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
-      <c r="B3" s="118"/>
-      <c r="C3" s="129" t="s">
-        <v>166</v>
+      <c r="B3" s="130"/>
+      <c r="C3" s="108" t="s">
+        <v>181</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
       <c r="E3" s="5"/>
-      <c r="F3" s="120"/>
-      <c r="G3" s="131" t="s">
-        <v>167</v>
-      </c>
-      <c r="H3" s="82" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F3" s="133"/>
+      <c r="G3" s="110" t="s">
+        <v>183</v>
+      </c>
+      <c r="H3" s="83" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="121.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
-      <c r="B4" s="119"/>
-      <c r="C4" s="128" t="s">
-        <v>169</v>
+      <c r="B4" s="131"/>
+      <c r="C4" s="107" t="s">
+        <v>185</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="F4" s="120"/>
-      <c r="G4" s="131" t="s">
-        <v>163</v>
-      </c>
-      <c r="H4" s="82" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="F4" s="133"/>
+      <c r="G4" s="110" t="s">
+        <v>175</v>
+      </c>
+      <c r="H4" s="83" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="F7" s="1" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
     </row>
   </sheetData>
@@ -5237,6 +5240,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010031C6D98A8BA9914F9CBD1D8D43561C2B" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="20dc68b959a60313fbcac393e99fd10f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7e1cd103-0302-4a32-9a4b-e115c950d959" xmlns:ns3="50b62f6a-6a2d-4510-bfe7-b1a3c00072e4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7195712bd1d9adc40779bc7b93adecf4" ns2:_="" ns3:_="">
     <xsd:import namespace="7e1cd103-0302-4a32-9a4b-e115c950d959"/>
@@ -5479,7 +5491,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="7e1cd103-0302-4a32-9a4b-e115c950d959">
@@ -5490,16 +5502,15 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D186559C-C381-484C-9B7A-F4466E79AE25}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C8A29AC-6BF1-4D4D-9282-8A0E51881B4F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5518,27 +5529,19 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D71C399E-D560-405D-A693-6A86DF1C82D7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="50b62f6a-6a2d-4510-bfe7-b1a3c00072e4"/>
     <ds:schemaRef ds:uri="7e1cd103-0302-4a32-9a4b-e115c950d959"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="50b62f6a-6a2d-4510-bfe7-b1a3c00072e4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D186559C-C381-484C-9B7A-F4466E79AE25}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>